<commit_message>
Sprint and gantt update
</commit_message>
<xml_diff>
--- a/SprintBacklog/Sprint3.xlsx
+++ b/SprintBacklog/Sprint3.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Database code</t>
-  </si>
-  <si>
-    <t>SPRINT UNSUCESSFUL - very ill during the first week  and then was on holiday 13th - 17th</t>
   </si>
   <si>
     <t>Mon 19th Jan 2015 - Mon 2nd Feb 2015</t>
@@ -229,7 +226,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="30">
     <dxf>
       <fill>
         <patternFill>
@@ -345,6 +342,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -352,6 +363,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -373,6 +391,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -388,90 +413,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -507,8 +448,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="37"/>
-      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -817,7 +758,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,16 +774,14 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="V3" s="7" t="s">
         <v>14</v>
       </c>
@@ -854,7 +793,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -924,9 +863,15 @@
       <c r="E6" s="8">
         <v>4</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="F6" s="8">
+        <v>4</v>
+      </c>
+      <c r="G6" s="8">
+        <v>4</v>
+      </c>
+      <c r="H6" s="8">
+        <v>4</v>
+      </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -945,7 +890,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="8">
         <v>15</v>
@@ -957,37 +902,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="8">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H7" s="8">
-        <v>15</v>
-      </c>
-      <c r="I7" s="8">
-        <v>15</v>
-      </c>
-      <c r="J7" s="8">
-        <v>15</v>
-      </c>
-      <c r="K7" s="8">
-        <v>15</v>
-      </c>
-      <c r="L7" s="8">
-        <v>15</v>
-      </c>
-      <c r="M7" s="8">
-        <v>15</v>
-      </c>
-      <c r="N7" s="8">
-        <v>15</v>
-      </c>
-      <c r="O7" s="8">
-        <v>15</v>
-      </c>
-      <c r="P7" s="8">
-        <v>15</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -1006,6 +924,15 @@
       <c r="E8" s="8">
         <v>3</v>
       </c>
+      <c r="F8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1015,7 +942,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="8">
         <v>20</v>
@@ -1024,40 +951,13 @@
         <v>20</v>
       </c>
       <c r="F9" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G9" s="8">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="H9" s="8">
-        <v>20</v>
-      </c>
-      <c r="I9" s="8">
-        <v>20</v>
-      </c>
-      <c r="J9" s="8">
-        <v>20</v>
-      </c>
-      <c r="K9" s="8">
-        <v>20</v>
-      </c>
-      <c r="L9" s="8">
-        <v>20</v>
-      </c>
-      <c r="M9" s="8">
-        <v>20</v>
-      </c>
-      <c r="N9" s="8">
-        <v>20</v>
-      </c>
-      <c r="O9" s="8">
-        <v>20</v>
-      </c>
-      <c r="P9" s="8">
-        <v>20</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
@@ -1080,7 +980,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -1355,99 +1255,99 @@
       </c>
       <c r="F20">
         <f>SUM(F4:F16)</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G20">
         <f>SUM(G4:G16)</f>
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="H20">
         <f>SUM(H4:H16)</f>
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="I20">
         <f>SUM(I4:I16)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <f>SUM(J4:J16)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <f>SUM(K4:K19)</f>
-        <v>35</v>
+        <f t="shared" ref="K20:Q20" si="0">SUM(K4:K19)</f>
+        <v>0</v>
       </c>
       <c r="L20">
-        <f>SUM(L4:L19)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="M20">
-        <f>SUM(M4:M19)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="N20">
-        <f>SUM(N4:N19)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="O20">
-        <f>SUM(O4:O19)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="P20">
-        <f>SUM(P4:P19)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <f>SUM(Q4:Q19)</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C18">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="31" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="32" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C18)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>